<commit_message>
Correção do bug entre as versões do Chromedriver e o driver. Implementação da nomenclatura correta, e ajuste da primeira classe de teste com o JUnit4
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriela.nomura\Documents\automacao\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0788B4E0-95ED-453D-9260-1DF000C3FBDA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6310954A-CB95-40DF-A9CA-3D3F1C99432D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C4985153-42DC-42E2-B000-666D3A9AB41B}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20760" windowHeight="11820" xr2:uid="{C4985153-42DC-42E2-B000-666D3A9AB41B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -463,7 +459,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>